<commit_message>
corrected some of my concepts names
</commit_message>
<xml_diff>
--- a/keyConcepts/toTest/Concepts.xlsx
+++ b/keyConcepts/toTest/Concepts.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Лист1" state="visible" r:id="rId3"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>относительные*:</t>
   </si>
@@ -34,9 +37,6 @@
     <t>диапазон значений*</t>
   </si>
   <si>
-    <t>value_diapazone</t>
-  </si>
-  <si>
     <t>компания-производитель</t>
   </si>
   <si>
@@ -49,12 +49,6 @@
     <t>лекарственная форма</t>
   </si>
   <si>
-    <t>medicament_form</t>
-  </si>
-  <si>
-    <t>dosage_form</t>
-  </si>
-  <si>
     <t>лекарственная форма*</t>
   </si>
   <si>
@@ -64,9 +58,6 @@
     <t>medicinal_agent</t>
   </si>
   <si>
-    <t>medicinal_product</t>
-  </si>
-  <si>
     <t>описание кода*</t>
   </si>
   <si>
@@ -151,8 +142,7 @@
     <t>торговое название*</t>
   </si>
   <si>
-    <t>
-единица лекарственной формы</t>
+    <t>единица лекарственной формы</t>
   </si>
   <si>
     <t>medicament_form_unit</t>
@@ -213,48 +203,49 @@
   </si>
   <si>
     <t>indications</t>
+  </si>
+  <si>
+    <t>medicinal_form</t>
+  </si>
+  <si>
+    <t>Глеб:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
       <i/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
       <i/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
       <i/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -262,9 +253,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -297,19 +286,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -357,343 +333,654 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="2" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="3" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="4" applyFont="1" fontId="2" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="5" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="6" applyFont="1" fontId="3" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+  <a:themeElements>
+    <a:clrScheme name="Стандартная">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Стандартная">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Стандартная">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="8.57"/>
-    <col min="2" customWidth="1" max="2" width="31.86"/>
-    <col min="3" customWidth="1" max="3" width="36.57"/>
-    <col min="4" customWidth="1" max="4" width="44.57"/>
-    <col min="5" customWidth="1" max="5" width="9.71"/>
-    <col min="6" customWidth="1" max="6" width="40.57"/>
-    <col min="7" customWidth="1" max="7" width="30.86"/>
-    <col min="8" customWidth="1" max="8" width="20.71"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="40.5703125" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c s="4" r="B1"/>
-      <c t="s" s="7" r="C1">
+    <row r="1" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B1" s="3"/>
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c s="1" r="D1"/>
-      <c s="4" r="E1"/>
-      <c t="s" s="5" r="F1">
+      <c r="D1" s="1"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
-      <c s="1" r="G1"/>
-    </row>
-    <row r="2">
-      <c t="s" s="6" r="C2">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="D2">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="6" r="F2">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="G2">
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c s="3" r="H2"/>
-    </row>
-    <row r="3">
-      <c t="s" s="3" r="B3">
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="C3">
-        <v>6</v>
-      </c>
-      <c t="s" r="D3">
+      <c r="F3" s="8" t="s">
         <v>7</v>
       </c>
-      <c t="s" r="F3">
+      <c r="G3" s="8" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="G3">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="2"/>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c s="3" r="H3"/>
-    </row>
-    <row r="4">
-      <c s="3" r="B4"/>
-      <c t="s" r="C4">
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>10</v>
       </c>
-      <c t="s" r="D4">
-        <v>9</v>
-      </c>
-      <c t="s" r="F4">
+      <c r="G4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="9"/>
+      <c r="C5" s="7" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="G4">
+      <c r="D5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c s="3" r="H4"/>
-    </row>
-    <row r="5">
-      <c t="s" s="3" r="B5">
+      <c r="G5" t="s">
         <v>13</v>
       </c>
-      <c t="s" r="C5">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="D5">
-        <v>12</v>
-      </c>
-      <c t="s" r="F5">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="G5">
+      <c r="F6" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="3" r="H5">
+      <c r="G6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6">
-      <c s="3" r="B6"/>
-      <c t="s" r="C6">
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="2"/>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c t="s" r="D6">
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c t="s" r="F6">
+      <c r="F7" t="s">
         <v>20</v>
       </c>
-      <c t="s" r="G6">
+      <c r="G7" t="s">
         <v>21</v>
       </c>
-      <c s="3" r="H6"/>
-    </row>
-    <row r="7">
-      <c s="3" r="B7"/>
-      <c t="s" r="C7">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="2"/>
+      <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="D7">
+      <c r="D8" t="s">
         <v>23</v>
       </c>
-      <c t="s" r="F7">
+      <c r="F8" t="s">
         <v>24</v>
       </c>
-      <c t="s" r="G7">
+      <c r="G8" t="s">
         <v>25</v>
       </c>
-      <c s="3" r="H7"/>
-    </row>
-    <row r="8">
-      <c s="3" r="B8"/>
-      <c t="s" r="C8">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="2"/>
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c t="s" r="D8">
+      <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c t="s" r="F8">
+      <c r="F9" t="s">
         <v>28</v>
       </c>
-      <c t="s" r="G8">
+      <c r="G9" t="s">
         <v>29</v>
       </c>
-      <c s="3" r="H8"/>
-    </row>
-    <row r="9">
-      <c s="3" r="B9"/>
-      <c t="s" r="C9">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="2"/>
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c t="s" r="D9">
+      <c r="D10" t="s">
         <v>31</v>
       </c>
-      <c t="s" r="F9">
+      <c r="F10" t="s">
         <v>32</v>
       </c>
-      <c t="s" r="G9">
+      <c r="H10" s="2" t="s">
         <v>33</v>
       </c>
-      <c s="3" r="H9"/>
-    </row>
-    <row r="10">
-      <c s="3" r="B10"/>
-      <c t="s" r="C10">
+    </row>
+    <row r="11" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
         <v>34</v>
       </c>
-      <c t="s" r="D10">
+      <c r="C11" t="s">
         <v>35</v>
       </c>
-      <c t="s" r="F10">
+      <c r="F11" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="3" r="H10">
+      <c r="G11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11">
-      <c t="s" s="3" r="B11">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
         <v>38</v>
       </c>
-      <c t="s" r="C11">
+      <c r="F12" t="s">
         <v>39</v>
       </c>
-      <c t="s" r="F11">
+      <c r="G12" t="s">
         <v>40</v>
       </c>
-      <c t="s" r="G11">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
         <v>41</v>
       </c>
-      <c s="3" r="H11"/>
-    </row>
-    <row customHeight="1" r="12" ht="3.75">
-      <c t="s" s="3" r="B12">
-        <v>37</v>
-      </c>
-      <c t="s" r="C12">
+      <c r="F13" t="s">
         <v>42</v>
       </c>
-      <c t="s" r="F12">
+      <c r="G13" t="s">
         <v>43</v>
       </c>
-      <c t="s" r="G12">
+      <c r="H13" s="2" t="s">
         <v>44</v>
       </c>
-      <c s="3" r="H12"/>
-    </row>
-    <row customHeight="1" r="13" ht="3.0">
-      <c t="s" s="3" r="B13">
-        <v>41</v>
-      </c>
-      <c t="s" r="C13">
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
         <v>45</v>
       </c>
-      <c t="s" r="F13">
+      <c r="C14" t="s">
         <v>46</v>
       </c>
-      <c t="s" r="G13">
+      <c r="F14" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="3" r="H13">
+      <c r="G14" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="14">
-      <c t="s" s="3" r="B14">
+      <c r="H14" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
         <v>49</v>
       </c>
-      <c t="s" r="C14">
+      <c r="C15" t="s">
         <v>50</v>
       </c>
-      <c t="s" r="F14">
+      <c r="D15" t="s">
         <v>51</v>
       </c>
-      <c t="s" r="G14">
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="3" r="H14">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15">
-      <c t="s" s="3" r="B15">
+      <c r="D16" t="s">
         <v>53</v>
       </c>
-      <c t="s" r="C15">
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
         <v>54</v>
       </c>
-      <c t="s" r="D15">
+      <c r="D17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16">
-      <c t="s" s="3" r="B16">
-        <v>53</v>
-      </c>
-      <c t="s" r="C16">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
         <v>56</v>
       </c>
-      <c t="s" r="D16">
+      <c r="D19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17">
-      <c t="s" s="3" r="B17">
-        <v>53</v>
-      </c>
-      <c t="s" r="C17">
+    <row r="20" spans="2:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
         <v>58</v>
       </c>
-      <c t="s" r="D17">
+      <c r="D20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19">
-      <c t="s" r="C19">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
         <v>60</v>
       </c>
-      <c t="s" r="D19">
+      <c r="C21" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="20">
-      <c t="s" r="C20">
+      <c r="D21" t="s">
         <v>62</v>
       </c>
-      <c t="s" r="D20">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21">
-      <c t="s" r="B21">
-        <v>64</v>
-      </c>
-      <c t="s" r="C21">
-        <v>65</v>
-      </c>
-      <c t="s" r="D21">
-        <v>66</v>
-      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>